<commit_message>
Progress studies using Kaon variables
</commit_message>
<xml_diff>
--- a/BDTData.xlsx
+++ b/BDTData.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chandler/Documents/PhD/Upstream/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3467EC-9FC0-6B46-88E3-1A5E913A1595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9900DF35-9C76-3A42-BFCB-704ACFF8DA3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="860" windowWidth="28040" windowHeight="16920" xr2:uid="{3253F664-ABEB-AD4A-9085-A3E06566AB20}"/>
+    <workbookView xWindow="760" yWindow="740" windowWidth="28040" windowHeight="16920" xr2:uid="{3253F664-ABEB-AD4A-9085-A3E06566AB20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>Model Name</t>
   </si>
@@ -117,6 +117,27 @@
   </si>
   <si>
     <t>pprich</t>
+  </si>
+  <si>
+    <t>Kaon2</t>
+  </si>
+  <si>
+    <t>rs1gtk3, pKaon</t>
+  </si>
+  <si>
+    <t>Kaon3</t>
+  </si>
+  <si>
+    <t>rs1gtk3, pKaon,gtk3x</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>Kaon4</t>
+  </si>
+  <si>
+    <t>pKaon,gtk3x,gtk3y</t>
   </si>
 </sst>
 </file>
@@ -175,9 +196,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -185,6 +203,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -523,7 +544,7 @@
   <dimension ref="D2:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -539,52 +560,52 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
     </row>
     <row r="4" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
     </row>
     <row r="5" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3" t="s">
+      <c r="H5" s="6"/>
+      <c r="I5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3" t="s">
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3" t="s">
+      <c r="M5" s="6"/>
+      <c r="N5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3" t="s">
+      <c r="O5" s="6"/>
+      <c r="P5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="Q5" s="3"/>
+      <c r="Q5" s="6"/>
     </row>
     <row r="6" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D6" s="2" t="s">
@@ -669,338 +690,405 @@
       </c>
     </row>
     <row r="8" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>2329</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <v>56</v>
       </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4">
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3">
         <v>0.82889999999999997</v>
       </c>
-      <c r="M8" s="4"/>
+      <c r="M8" s="3"/>
       <c r="N8" s="1">
         <v>56</v>
       </c>
       <c r="O8" s="1">
         <v>0</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="P8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q8" s="4" t="s">
+      <c r="Q8" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>0.99</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>2313</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="4">
         <v>69</v>
       </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4">
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3">
         <v>0.86350000000000005</v>
       </c>
-      <c r="M9" s="4"/>
+      <c r="M9" s="3"/>
       <c r="N9" s="1">
         <v>55</v>
       </c>
       <c r="O9" s="1">
         <v>0</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="P9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q9" s="4" t="s">
+      <c r="Q9" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>0.99299999999999999</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>2195</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="4">
         <v>63</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4">
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3">
         <v>0.83069999999999999</v>
       </c>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4">
+      <c r="M10" s="3"/>
+      <c r="N10" s="3">
         <v>45</v>
       </c>
-      <c r="O10" s="4">
+      <c r="O10" s="3">
         <v>0</v>
       </c>
-      <c r="P10" s="4" t="s">
+      <c r="P10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q10" s="4" t="s">
+      <c r="Q10" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>0.99399999999999999</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>2137</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <v>58</v>
       </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="5">
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="4">
         <v>0.8135</v>
       </c>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4">
+      <c r="M11" s="3"/>
+      <c r="N11" s="3">
         <v>39</v>
       </c>
-      <c r="O11" s="4">
+      <c r="O11" s="3">
         <v>0</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="P11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q11" s="4" t="s">
+      <c r="Q11" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>0.99299999999999999</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <v>2165</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="3">
         <v>58</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4">
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3">
         <v>0.82989999999999997</v>
       </c>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4">
+      <c r="M12" s="3"/>
+      <c r="N12" s="3">
         <v>46</v>
       </c>
-      <c r="O12" s="4">
+      <c r="O12" s="3">
         <v>0</v>
       </c>
-      <c r="P12" s="4" t="s">
+      <c r="P12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q12" s="4" t="s">
+      <c r="Q12" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-    </row>
     <row r="14" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
     </row>
     <row r="15" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
+      <c r="D15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="3">
+        <v>2302</v>
+      </c>
+      <c r="H15" s="3">
+        <v>56</v>
+      </c>
+      <c r="I15" s="3">
+        <v>18699</v>
+      </c>
+      <c r="J15" s="3">
+        <v>3152</v>
+      </c>
+      <c r="K15" s="3">
+        <v>8543</v>
+      </c>
+      <c r="L15" s="3">
+        <v>0.83460000000000001</v>
+      </c>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
     </row>
     <row r="16" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
+      <c r="D16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="G16" s="3">
+        <v>2233</v>
+      </c>
+      <c r="H16" s="3">
+        <v>57</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L16" s="3">
+        <v>0.83940000000000003</v>
+      </c>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
     </row>
     <row r="17" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
+      <c r="D17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="G17" s="3">
+        <v>2113</v>
+      </c>
+      <c r="H17" s="3">
+        <v>54</v>
+      </c>
+      <c r="I17" s="3">
+        <v>17143</v>
+      </c>
+      <c r="J17" s="3">
+        <v>2952</v>
+      </c>
+      <c r="K17" s="3">
+        <v>8372</v>
+      </c>
+      <c r="L17" s="3">
+        <v>0.84830000000000005</v>
+      </c>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
     </row>
     <row r="18" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
+      <c r="D18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="G18" s="3">
+        <v>2041</v>
+      </c>
+      <c r="H18" s="3">
+        <v>47</v>
+      </c>
+      <c r="I18" s="3">
+        <v>17731</v>
+      </c>
+      <c r="J18" s="3">
+        <v>2927</v>
+      </c>
+      <c r="K18" s="3">
+        <v>8440</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0.86780000000000002</v>
+      </c>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
     </row>
     <row r="19" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
     </row>
     <row r="20" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
     </row>
     <row r="21" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
     </row>
     <row r="22" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
     </row>
     <row r="23" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3">
+        <f>(I17-I15)/I15</f>
+        <v>-8.3213006043103915E-2</v>
+      </c>
+      <c r="J23" s="3">
+        <f>(J17-J15)/J15</f>
+        <v>-6.3451776649746189E-2</v>
+      </c>
+      <c r="K23" s="3">
+        <f>(K17-K15)/K15</f>
+        <v>-2.0016387685824651E-2</v>
+      </c>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
     </row>
     <row r="24" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D24" s="1"/>

</xml_diff>

<commit_message>
Major updates to analysis
</commit_message>
<xml_diff>
--- a/BDTData.xlsx
+++ b/BDTData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chandler/Documents/PhD/Upstream/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9900DF35-9C76-3A42-BFCB-704ACFF8DA3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904A2CAC-41CD-724E-BA04-32F36438A1B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="740" windowWidth="28040" windowHeight="16920" xr2:uid="{3253F664-ABEB-AD4A-9085-A3E06566AB20}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16920" xr2:uid="{3253F664-ABEB-AD4A-9085-A3E06566AB20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
   <si>
     <t>Model Name</t>
   </si>
@@ -138,13 +138,31 @@
   </si>
   <si>
     <t>pKaon,gtk3x,gtk3y</t>
+  </si>
+  <si>
+    <t>Kaon5</t>
+  </si>
+  <si>
+    <t>^+ExtraHitsWord</t>
+  </si>
+  <si>
+    <t>Same w/o hits veto applied such that BDT absorbs the veto</t>
+  </si>
+  <si>
+    <t>TMVA No GTK Extra Hits</t>
+  </si>
+  <si>
+    <t>One of these two rows HAS to be wrong -- sampleC, maybe I typed the stuff the wrong way</t>
+  </si>
+  <si>
+    <t>Ke4 not tested for Kaon5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -161,6 +179,19 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -187,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -201,11 +232,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -541,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBCABC4D-7303-5444-97C3-4EF78276C471}">
-  <dimension ref="D2:Q24"/>
+  <dimension ref="D2:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="109" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -560,52 +603,52 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
     </row>
     <row r="5" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6" t="s">
+      <c r="H5" s="8"/>
+      <c r="I5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6" t="s">
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6" t="s">
+      <c r="M5" s="8"/>
+      <c r="N5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6" t="s">
+      <c r="O5" s="8"/>
+      <c r="P5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="Q5" s="6"/>
+      <c r="Q5" s="8"/>
     </row>
     <row r="6" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D6" s="2" t="s">
@@ -947,7 +990,7 @@
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
     </row>
-    <row r="17" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D17" s="3" t="s">
         <v>29</v>
       </c>
@@ -979,7 +1022,7 @@
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
     </row>
-    <row r="18" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D18" s="3" t="s">
         <v>32</v>
       </c>
@@ -1011,99 +1054,150 @@
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
     </row>
-    <row r="19" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
+    <row r="19" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.995</v>
+      </c>
+      <c r="G19" s="10">
+        <v>1807</v>
+      </c>
+      <c r="H19" s="10">
+        <v>31</v>
+      </c>
+      <c r="I19" s="3">
+        <v>18200</v>
+      </c>
+      <c r="J19" s="3">
+        <v>2974</v>
+      </c>
+      <c r="K19" s="3">
+        <v>8439</v>
+      </c>
+      <c r="L19" s="3">
+        <v>0.90069999999999995</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="N19" s="6"/>
       <c r="O19" s="3"/>
     </row>
-    <row r="20" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
+    <row r="20" spans="4:16" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="10">
+        <v>1828</v>
+      </c>
+      <c r="H20" s="10">
+        <v>31</v>
+      </c>
+      <c r="I20" s="3">
+        <v>18399</v>
+      </c>
+      <c r="J20" s="3">
+        <v>2978</v>
+      </c>
+      <c r="K20" s="3">
+        <v>8533</v>
+      </c>
+      <c r="L20" s="3">
+        <v>0.90069999999999995</v>
+      </c>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
       <c r="O20" s="3"/>
-    </row>
-    <row r="21" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
+      <c r="P20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D21" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="10">
+        <v>2366</v>
+      </c>
+      <c r="H21" s="10">
+        <v>60</v>
+      </c>
+      <c r="I21" s="3">
+        <v>18942</v>
+      </c>
+      <c r="J21" s="3">
+        <v>3165</v>
+      </c>
+      <c r="K21" s="3">
+        <v>8653</v>
+      </c>
+      <c r="L21" s="3">
+        <v>0.83460000000000001</v>
+      </c>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
     </row>
-    <row r="22" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
     </row>
-    <row r="23" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="3">
-        <f>(I17-I15)/I15</f>
-        <v>-8.3213006043103915E-2</v>
-      </c>
-      <c r="J23" s="3">
-        <f>(J17-J15)/J15</f>
-        <v>-6.3451776649746189E-2</v>
-      </c>
-      <c r="K23" s="3">
-        <f>(K17-K15)/K15</f>
-        <v>-2.0016387685824651E-2</v>
-      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
     </row>
-    <row r="24" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="4:16" x14ac:dyDescent="0.2">
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
     </row>
+    <row r="25" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="10">
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="M19:N20"/>
+    <mergeCell ref="E20:F20"/>
     <mergeCell ref="D2:H3"/>
     <mergeCell ref="I5:K5"/>
     <mergeCell ref="P5:Q5"/>
@@ -1113,5 +1207,6 @@
     <mergeCell ref="N5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>